<commit_message>
#114-Introduce Remarks column on Sales Per customer report. Minor UI enhancements on Reports details page
</commit_message>
<xml_diff>
--- a/Beelina.API/Templates/ReportTemplates/SalesPerCustomerReport_Template.xlsx
+++ b/Beelina.API/Templates/ReportTemplates/SalesPerCustomerReport_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Beelina\Beelina.API\Templates\ReportTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Beelina1\Beelina\Beelina.API\Templates\ReportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E981A7-D7F8-433E-93FD-BE3B6F5F0A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEC5A74-2428-4FD7-99E7-8CA22FAE8FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E006132D-31D5-4210-A706-5BCB02CE16A0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Customer</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Bad Order</t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -97,7 +100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -106,6 +109,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B87709B-2F56-417A-A5BA-952D47A78533}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,9 +440,10 @@
     <col min="4" max="4" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="3"/>
+    <col min="7" max="7" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,6 +461,9 @@
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>